<commit_message>
fix bug siswa dan rombel
</commit_message>
<xml_diff>
--- a/downloads/template_siswa.xlsx
+++ b/downloads/template_siswa.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\siakad\downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050"/>
   </bookViews>
@@ -91,9 +96,6 @@
     <t>penghasilan wali</t>
   </si>
   <si>
-    <t>telp siswa</t>
-  </si>
-  <si>
     <t>telp ayah</t>
   </si>
   <si>
@@ -101,6 +103,9 @@
   </si>
   <si>
     <t>tanggal masuk</t>
+  </si>
+  <si>
+    <t>telp wali</t>
   </si>
 </sst>
 </file>
@@ -147,6 +152,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -195,7 +203,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -230,7 +238,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -441,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +532,7 @@
         <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AA1" t="s">
         <v>25</v>
@@ -533,7 +541,7 @@
         <v>26</v>
       </c>
       <c r="AC1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -564,9 +572,9 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="pekerjaan wali" sqref="X1:X1048576"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="penghasilan wali" sqref="Y1:Y1048576"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="tanggal masuk" sqref="Z1:Z1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="telp siswa" sqref="AA1:AA1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="telp ayah" sqref="AB1:AB1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="telp ibu" sqref="AC1:AC1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="telp wali" sqref="AC1:AC1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="telp ayah" sqref="AA1:AA1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="telp ibu" sqref="AB1:AB1048576"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>